<commit_message>
Final Project - submission
</commit_message>
<xml_diff>
--- a/Battle Pets/Assets/Data/AbilitySheet.xlsx
+++ b/Battle Pets/Assets/Data/AbilitySheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\GAM111 - Battle Pets\BattlePets\Assets\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\BattlePets\Battle Pets\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,7 +491,7 @@
         <v>20</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>16</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -525,7 +525,7 @@
         <v>24</v>
       </c>
       <c r="E5">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
         <v>33</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>20</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>16</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -593,7 +593,7 @@
         <v>20</v>
       </c>
       <c r="E9">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -610,7 +610,7 @@
         <v>28</v>
       </c>
       <c r="E10">
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>20</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>25</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,7 +678,7 @@
         <v>12</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
         <v>20</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>14</v>
       </c>
       <c r="E17">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>